<commit_message>
Added Conception for pre development
Visio sketch added / interaction between ERP & App modules
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Burndown Chart.xlsx
+++ b/Gestion de Projet/Burndown Chart.xlsx
@@ -474,14 +474,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2327,163 +2327,163 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6224,8 +6224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7458,7 +7458,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" s="9">
         <f t="shared" si="5"/>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="L58" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="7:12" x14ac:dyDescent="0.25">
@@ -7478,7 +7478,7 @@
         <v>5</v>
       </c>
       <c r="J59" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K59" s="9">
         <f t="shared" si="5"/>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="L59" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="7:12" x14ac:dyDescent="0.25">
@@ -7498,7 +7498,7 @@
         <v>7</v>
       </c>
       <c r="J60" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K60" s="9">
         <f t="shared" si="5"/>
@@ -7506,7 +7506,7 @@
       </c>
       <c r="L60" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="7:12" x14ac:dyDescent="0.25">
@@ -7518,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K61" s="9">
         <f t="shared" si="5"/>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="L61" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="7:12" x14ac:dyDescent="0.25">
@@ -7538,7 +7538,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" s="9">
         <f t="shared" si="5"/>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="L62" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="7:12" x14ac:dyDescent="0.25">
@@ -7566,7 +7566,7 @@
       </c>
       <c r="L63" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="7:12" x14ac:dyDescent="0.25">
@@ -7586,7 +7586,7 @@
       </c>
       <c r="L64" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
@@ -7606,7 +7606,7 @@
       </c>
       <c r="L65" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
@@ -7626,7 +7626,7 @@
       </c>
       <c r="L66" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
@@ -7646,7 +7646,7 @@
       </c>
       <c r="L67" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
@@ -7666,7 +7666,7 @@
       </c>
       <c r="L68" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
@@ -7686,7 +7686,7 @@
       </c>
       <c r="L69" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
@@ -7718,7 +7718,7 @@
       </c>
       <c r="L70" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
@@ -7750,7 +7750,7 @@
       </c>
       <c r="L71" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
@@ -7782,7 +7782,7 @@
       </c>
       <c r="L72" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
@@ -7814,7 +7814,7 @@
       </c>
       <c r="L73" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
@@ -7846,7 +7846,7 @@
       </c>
       <c r="L74" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
@@ -7878,7 +7878,7 @@
       </c>
       <c r="L75" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
@@ -7910,7 +7910,7 @@
       </c>
       <c r="L76" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
@@ -7942,7 +7942,7 @@
       </c>
       <c r="L77" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
@@ -7974,7 +7974,7 @@
       </c>
       <c r="L78" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
@@ -8006,7 +8006,7 @@
       </c>
       <c r="L79" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">
@@ -8038,7 +8038,7 @@
       </c>
       <c r="L80" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
@@ -8070,7 +8070,7 @@
       </c>
       <c r="L81" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="L82" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
@@ -8134,7 +8134,7 @@
       </c>
       <c r="L83" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
@@ -8166,7 +8166,7 @@
       </c>
       <c r="L84" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
@@ -8198,7 +8198,7 @@
       </c>
       <c r="L85" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
@@ -8230,7 +8230,7 @@
       </c>
       <c r="L86" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
@@ -8262,7 +8262,7 @@
       </c>
       <c r="L87" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="L88" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
@@ -8326,7 +8326,7 @@
       </c>
       <c r="L89" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
@@ -8358,7 +8358,7 @@
       </c>
       <c r="L90" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -8390,7 +8390,7 @@
       </c>
       <c r="L91" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
@@ -8410,7 +8410,7 @@
       </c>
       <c r="L92" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
@@ -8430,7 +8430,7 @@
       </c>
       <c r="L93" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
@@ -8450,7 +8450,7 @@
       </c>
       <c r="L94" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
@@ -8470,7 +8470,7 @@
       </c>
       <c r="L95" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
@@ -8490,7 +8490,7 @@
       </c>
       <c r="L96" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="7:12" x14ac:dyDescent="0.25">
@@ -8510,7 +8510,7 @@
       </c>
       <c r="L97" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="7:12" x14ac:dyDescent="0.25">
@@ -8530,7 +8530,7 @@
       </c>
       <c r="L98" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="7:12" x14ac:dyDescent="0.25">
@@ -8550,7 +8550,7 @@
       </c>
       <c r="L99" s="9">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="7:12" x14ac:dyDescent="0.25">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="L100" s="9">
         <f t="shared" ref="L100:L104" si="8">L99-J100</f>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="7:12" x14ac:dyDescent="0.25">
@@ -8590,7 +8590,7 @@
       </c>
       <c r="L101" s="9">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="7:12" x14ac:dyDescent="0.25">
@@ -8610,7 +8610,7 @@
       </c>
       <c r="L102" s="9">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="7:12" x14ac:dyDescent="0.25">
@@ -8630,7 +8630,7 @@
       </c>
       <c r="L103" s="9">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="7:12" x14ac:dyDescent="0.25">
@@ -8650,7 +8650,7 @@
       </c>
       <c r="L104" s="9">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="7:12" x14ac:dyDescent="0.25">
@@ -8670,7 +8670,7 @@
       </c>
       <c r="L105" s="9">
         <f t="shared" ref="L105:L110" si="10">L104-J105</f>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="7:12" x14ac:dyDescent="0.25">
@@ -8690,7 +8690,7 @@
       </c>
       <c r="L106" s="9">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="7:12" x14ac:dyDescent="0.25">
@@ -8710,7 +8710,7 @@
       </c>
       <c r="L107" s="9">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="7:12" x14ac:dyDescent="0.25">
@@ -8730,7 +8730,7 @@
       </c>
       <c r="L108" s="9">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="7:12" x14ac:dyDescent="0.25">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="L109" s="9">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="7:12" x14ac:dyDescent="0.25">
@@ -8770,26 +8770,26 @@
       </c>
       <c r="L110" s="9">
         <f t="shared" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G127" s="25" t="s">
+      <c r="G127" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H127" s="25"/>
-      <c r="I127" s="26" t="s">
+      <c r="H127" s="26"/>
+      <c r="I127" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="J127" s="26"/>
-      <c r="K127" s="26" t="s">
+      <c r="J127" s="24"/>
+      <c r="K127" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L127" s="26"/>
+      <c r="L127" s="24"/>
     </row>
     <row r="128" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G128" s="25"/>
-      <c r="H128" s="25"/>
+      <c r="G128" s="26"/>
+      <c r="H128" s="26"/>
       <c r="I128" s="10" t="s">
         <v>28</v>
       </c>
@@ -8818,12 +8818,12 @@
       </c>
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B130" s="24" t="s">
+      <c r="B130" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C130" s="24"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="24"/>
+      <c r="C130" s="25"/>
+      <c r="D130" s="25"/>
+      <c r="E130" s="25"/>
       <c r="G130" s="11">
         <v>43049</v>
       </c>
@@ -9613,6 +9613,16 @@
     </row>
   </sheetData>
   <mergeCells count="144">
+    <mergeCell ref="G148:H148"/>
+    <mergeCell ref="G149:H149"/>
+    <mergeCell ref="G140:H140"/>
+    <mergeCell ref="G141:H141"/>
+    <mergeCell ref="G142:H142"/>
+    <mergeCell ref="G143:H143"/>
+    <mergeCell ref="G144:H144"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="G127:H128"/>
+    <mergeCell ref="G129:H129"/>
     <mergeCell ref="G135:H135"/>
     <mergeCell ref="G136:H136"/>
     <mergeCell ref="G137:H137"/>
@@ -9622,15 +9632,6 @@
     <mergeCell ref="G131:H131"/>
     <mergeCell ref="G146:H146"/>
     <mergeCell ref="G147:H147"/>
-    <mergeCell ref="G148:H148"/>
-    <mergeCell ref="G149:H149"/>
-    <mergeCell ref="G140:H140"/>
-    <mergeCell ref="G141:H141"/>
-    <mergeCell ref="G142:H142"/>
-    <mergeCell ref="G143:H143"/>
-    <mergeCell ref="G144:H144"/>
-    <mergeCell ref="B130:E130"/>
-    <mergeCell ref="G127:H128"/>
     <mergeCell ref="I127:J127"/>
     <mergeCell ref="K127:L127"/>
     <mergeCell ref="G51:H51"/>
@@ -9650,13 +9651,11 @@
     <mergeCell ref="G84:H84"/>
     <mergeCell ref="G85:H85"/>
     <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G129:H129"/>
     <mergeCell ref="G64:H64"/>
     <mergeCell ref="G65:H65"/>
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="G67:H67"/>
     <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G87:H87"/>
     <mergeCell ref="G88:H88"/>
     <mergeCell ref="G79:H79"/>
     <mergeCell ref="G80:H80"/>
@@ -9733,6 +9732,7 @@
     <mergeCell ref="G71:H71"/>
     <mergeCell ref="G72:H72"/>
     <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G87:H87"/>
     <mergeCell ref="G156:H156"/>
     <mergeCell ref="G157:H157"/>
     <mergeCell ref="G158:H158"/>

</xml_diff>